<commit_message>
connect fire and main packages, ready for extracting fluxes, rates
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,9 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>particle_block-59</t>
+  </si>
+  <si>
+    <t>M/Z/O/E</t>
+  </si>
+  <si>
+    <t>MIXT,</t>
+  </si>
+  <si>
+    <t>O16</t>
+  </si>
+  <si>
+    <t>N14</t>
   </si>
   <si>
     <t>particle_block-137</t>
@@ -55,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,18 +364,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="4" width="9.140625"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:7">
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
         <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.37042E-17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.33158</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6.29018E-20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>14.2801</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.43272E-19</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.297053</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6.10277E-23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>13.8157</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>99.9999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.34609E-17</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.331988</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6.28408E-20</v>
+      </c>
+      <c r="D20" s="1">
+        <v>14.2806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>